<commit_message>
Removal of previous results
</commit_message>
<xml_diff>
--- a/Industry_User_Interface_v1.xlsx
+++ b/Industry_User_Interface_v1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\OneDrive - University of Nottingham Malaysia\The University of Nottingham\BC COP26 Trilateral Research Initiative\BCCOP26 Software Framework\Indutrial Case_v1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\OneDrive - University of Nottingham Malaysia\The University of Nottingham\BC COP26 Trilateral Research Initiative\BCCOP26TrilateralProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432AB481-7419-458C-B66E-69965551D4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C59AAEB-6875-42C4-B1F1-335421708742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,12 +30,6 @@
     <sheet name="NET_CI_DATA" sheetId="15" r:id="rId15"/>
     <sheet name="NET_COST_DATA" sheetId="16" r:id="rId16"/>
     <sheet name="TECH_IMPLEMENTATION_TIME" sheetId="17" r:id="rId17"/>
-    <sheet name="Results_Period_1" sheetId="18" r:id="rId18"/>
-    <sheet name="Results_Period_2" sheetId="19" r:id="rId19"/>
-    <sheet name="Results_Period_3" sheetId="20" r:id="rId20"/>
-    <sheet name="Results_Period_4" sheetId="21" r:id="rId21"/>
-    <sheet name="Results_Period_5" sheetId="22" r:id="rId22"/>
-    <sheet name="Results_Period_6" sheetId="23" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="276">
   <si>
     <t>CO2 Emissions / million t</t>
   </si>
@@ -881,45 +875,6 @@
   </si>
   <si>
     <t>TABLE 14: TECHNOLOGY IMPLEMENTATION TIME</t>
-  </si>
-  <si>
-    <t>Energy Generation</t>
-  </si>
-  <si>
-    <t>Gross Energy (TWh/y)</t>
-  </si>
-  <si>
-    <t>CO2 Intensity (Mt/TWh)</t>
-  </si>
-  <si>
-    <t>CCS_1 Selection</t>
-  </si>
-  <si>
-    <t>CCS_1 Ret (TWh/y)</t>
-  </si>
-  <si>
-    <t>Gas_2 Selection</t>
-  </si>
-  <si>
-    <t>GAS_2 (TWh/y)</t>
-  </si>
-  <si>
-    <t>Net Energy (TWh/y)</t>
-  </si>
-  <si>
-    <t>CO2 Load (Mt/y)</t>
-  </si>
-  <si>
-    <t>Total Cost (mil USD/y)</t>
-  </si>
-  <si>
-    <t>EP_NET_3</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>BECCS</t>
   </si>
 </sst>
 </file>
@@ -930,7 +885,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -967,12 +922,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1019,7 +968,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1349,27 +1298,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1550,12 +1484,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5145,12 +5073,6 @@
     <row r="28" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
@@ -5158,6 +5080,12 @@
     <mergeCell ref="A19:R19"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B21:R26" xr:uid="{00000000-0002-0000-1000-000000000000}">
@@ -5166,684 +5094,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:L12"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="15.85546875" style="42"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="69" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" s="69" t="s">
-        <v>276</v>
-      </c>
-      <c r="D1" s="69" t="s">
-        <v>277</v>
-      </c>
-      <c r="E1" s="69" t="s">
-        <v>278</v>
-      </c>
-      <c r="F1" s="69" t="s">
-        <v>279</v>
-      </c>
-      <c r="G1" s="69" t="s">
-        <v>280</v>
-      </c>
-      <c r="H1" s="69" t="s">
-        <v>281</v>
-      </c>
-      <c r="I1" s="69" t="s">
-        <v>282</v>
-      </c>
-      <c r="J1" s="69" t="s">
-        <v>283</v>
-      </c>
-      <c r="K1" s="69" t="s">
-        <v>284</v>
-      </c>
-      <c r="L1" s="69" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="68" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="42">
-        <v>0</v>
-      </c>
-      <c r="D2" s="42">
-        <v>0</v>
-      </c>
-      <c r="E2" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="F2" s="42">
-        <v>0</v>
-      </c>
-      <c r="G2" s="42">
-        <v>0</v>
-      </c>
-      <c r="H2" s="42">
-        <v>0</v>
-      </c>
-      <c r="I2" s="42">
-        <v>0</v>
-      </c>
-      <c r="J2" s="42">
-        <v>0</v>
-      </c>
-      <c r="K2" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="68" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="42">
-        <v>0</v>
-      </c>
-      <c r="D3" s="42">
-        <v>0</v>
-      </c>
-      <c r="E3" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="F3" s="42">
-        <v>0</v>
-      </c>
-      <c r="G3" s="42">
-        <v>0</v>
-      </c>
-      <c r="H3" s="42">
-        <v>0</v>
-      </c>
-      <c r="I3" s="42">
-        <v>0</v>
-      </c>
-      <c r="J3" s="42">
-        <v>0</v>
-      </c>
-      <c r="K3" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="68" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="42">
-        <v>0</v>
-      </c>
-      <c r="D4" s="42">
-        <v>0</v>
-      </c>
-      <c r="E4" s="42">
-        <v>0.15</v>
-      </c>
-      <c r="F4" s="42">
-        <v>0</v>
-      </c>
-      <c r="G4" s="42">
-        <v>0</v>
-      </c>
-      <c r="H4" s="42">
-        <v>0</v>
-      </c>
-      <c r="I4" s="42">
-        <v>0</v>
-      </c>
-      <c r="J4" s="42">
-        <v>0</v>
-      </c>
-      <c r="K4" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="68" t="s">
-        <v>112</v>
-      </c>
-      <c r="B5" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="42">
-        <v>0</v>
-      </c>
-      <c r="D5" s="42">
-        <v>0</v>
-      </c>
-      <c r="E5" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="F5" s="42">
-        <v>0</v>
-      </c>
-      <c r="G5" s="42">
-        <v>0</v>
-      </c>
-      <c r="H5" s="42">
-        <v>0</v>
-      </c>
-      <c r="I5" s="42">
-        <v>0</v>
-      </c>
-      <c r="J5" s="42">
-        <v>0</v>
-      </c>
-      <c r="K5" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="42">
-        <v>1</v>
-      </c>
-      <c r="D6" s="42">
-        <v>10</v>
-      </c>
-      <c r="E6" s="42">
-        <v>0.8</v>
-      </c>
-      <c r="F6" s="42">
-        <v>0</v>
-      </c>
-      <c r="G6" s="42">
-        <v>0</v>
-      </c>
-      <c r="H6" s="42">
-        <v>0</v>
-      </c>
-      <c r="I6" s="42">
-        <v>0</v>
-      </c>
-      <c r="J6" s="42">
-        <v>10</v>
-      </c>
-      <c r="K6" s="42">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="68" t="s">
-        <v>288</v>
-      </c>
-      <c r="B7" s="42" t="s">
-        <v>288</v>
-      </c>
-      <c r="C7" s="42">
-        <v>0</v>
-      </c>
-      <c r="E7" s="42">
-        <v>-1.2</v>
-      </c>
-      <c r="J7" s="42">
-        <v>0</v>
-      </c>
-      <c r="K7" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="68" t="s">
-        <v>162</v>
-      </c>
-      <c r="B8" s="42" t="s">
-        <v>162</v>
-      </c>
-      <c r="C8" s="42">
-        <v>1</v>
-      </c>
-      <c r="E8" s="42">
-        <v>0.6</v>
-      </c>
-      <c r="J8" s="42">
-        <v>10</v>
-      </c>
-      <c r="K8" s="42">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="42">
-        <v>0</v>
-      </c>
-      <c r="E9" s="42">
-        <v>0.15</v>
-      </c>
-      <c r="J9" s="42">
-        <v>0</v>
-      </c>
-      <c r="K9" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="68" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="42">
-        <v>0</v>
-      </c>
-      <c r="E10" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="J10" s="42">
-        <v>0</v>
-      </c>
-      <c r="K10" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="68" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="42">
-        <v>0</v>
-      </c>
-      <c r="E11" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="J11" s="42">
-        <v>0</v>
-      </c>
-      <c r="K11" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="68" t="s">
-        <v>287</v>
-      </c>
-      <c r="K12" s="42">
-        <v>14</v>
-      </c>
-      <c r="L12" s="42">
-        <v>1652.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:L12"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="15.7109375" style="42"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="69" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" s="69" t="s">
-        <v>276</v>
-      </c>
-      <c r="D1" s="69" t="s">
-        <v>277</v>
-      </c>
-      <c r="E1" s="69" t="s">
-        <v>278</v>
-      </c>
-      <c r="F1" s="69" t="s">
-        <v>279</v>
-      </c>
-      <c r="G1" s="69" t="s">
-        <v>280</v>
-      </c>
-      <c r="H1" s="69" t="s">
-        <v>281</v>
-      </c>
-      <c r="I1" s="69" t="s">
-        <v>282</v>
-      </c>
-      <c r="J1" s="69" t="s">
-        <v>283</v>
-      </c>
-      <c r="K1" s="69" t="s">
-        <v>284</v>
-      </c>
-      <c r="L1" s="69" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="68" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="42">
-        <v>0</v>
-      </c>
-      <c r="D2" s="42">
-        <v>0</v>
-      </c>
-      <c r="E2" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="F2" s="42">
-        <v>0</v>
-      </c>
-      <c r="G2" s="42">
-        <v>0</v>
-      </c>
-      <c r="H2" s="42">
-        <v>0</v>
-      </c>
-      <c r="I2" s="42">
-        <v>0</v>
-      </c>
-      <c r="J2" s="42">
-        <v>0</v>
-      </c>
-      <c r="K2" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="68" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="42">
-        <v>0</v>
-      </c>
-      <c r="D3" s="42">
-        <v>0</v>
-      </c>
-      <c r="E3" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="F3" s="42">
-        <v>0</v>
-      </c>
-      <c r="G3" s="42">
-        <v>0</v>
-      </c>
-      <c r="H3" s="42">
-        <v>0</v>
-      </c>
-      <c r="I3" s="42">
-        <v>0</v>
-      </c>
-      <c r="J3" s="42">
-        <v>0</v>
-      </c>
-      <c r="K3" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="68" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="42">
-        <v>0</v>
-      </c>
-      <c r="D4" s="42">
-        <v>0</v>
-      </c>
-      <c r="E4" s="42">
-        <v>0.15</v>
-      </c>
-      <c r="F4" s="42">
-        <v>0</v>
-      </c>
-      <c r="G4" s="42">
-        <v>0</v>
-      </c>
-      <c r="H4" s="42">
-        <v>0</v>
-      </c>
-      <c r="I4" s="42">
-        <v>0</v>
-      </c>
-      <c r="J4" s="42">
-        <v>0</v>
-      </c>
-      <c r="K4" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="68" t="s">
-        <v>112</v>
-      </c>
-      <c r="B5" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="42">
-        <v>1</v>
-      </c>
-      <c r="D5" s="42">
-        <v>5.28</v>
-      </c>
-      <c r="E5" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="F5" s="42">
-        <v>0</v>
-      </c>
-      <c r="G5" s="42">
-        <v>0</v>
-      </c>
-      <c r="H5" s="42">
-        <v>1</v>
-      </c>
-      <c r="I5" s="42">
-        <v>2.09</v>
-      </c>
-      <c r="J5" s="42">
-        <v>5.28</v>
-      </c>
-      <c r="K5" s="42">
-        <v>2.2200000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="42">
-        <v>1</v>
-      </c>
-      <c r="D6" s="42">
-        <v>14.72</v>
-      </c>
-      <c r="E6" s="42">
-        <v>0.8</v>
-      </c>
-      <c r="F6" s="42">
-        <v>0</v>
-      </c>
-      <c r="G6" s="42">
-        <v>0</v>
-      </c>
-      <c r="H6" s="42">
-        <v>0</v>
-      </c>
-      <c r="I6" s="42">
-        <v>0</v>
-      </c>
-      <c r="J6" s="42">
-        <v>14.72</v>
-      </c>
-      <c r="K6" s="42">
-        <v>11.78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="68" t="s">
-        <v>286</v>
-      </c>
-      <c r="B7" s="42" t="s">
-        <v>286</v>
-      </c>
-      <c r="C7" s="42">
-        <v>0</v>
-      </c>
-      <c r="E7" s="42">
-        <v>-1.2</v>
-      </c>
-      <c r="J7" s="42">
-        <v>0</v>
-      </c>
-      <c r="K7" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="68" t="s">
-        <v>162</v>
-      </c>
-      <c r="B8" s="42" t="s">
-        <v>162</v>
-      </c>
-      <c r="C8" s="42">
-        <v>1</v>
-      </c>
-      <c r="E8" s="42">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="J8" s="42">
-        <v>20</v>
-      </c>
-      <c r="K8" s="42">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="42">
-        <v>0</v>
-      </c>
-      <c r="E9" s="42">
-        <v>0.15</v>
-      </c>
-      <c r="J9" s="42">
-        <v>0</v>
-      </c>
-      <c r="K9" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="68" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="42">
-        <v>0</v>
-      </c>
-      <c r="E10" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="J10" s="42">
-        <v>0</v>
-      </c>
-      <c r="K10" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="68" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="42">
-        <v>0</v>
-      </c>
-      <c r="E11" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="J11" s="42">
-        <v>0</v>
-      </c>
-      <c r="K11" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="68" t="s">
-        <v>287</v>
-      </c>
-      <c r="K12" s="42">
-        <v>25</v>
-      </c>
-      <c r="L12" s="42">
-        <v>3100.49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -6361,1362 +5611,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:L12"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="15.7109375" style="42"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="69" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" s="69" t="s">
-        <v>276</v>
-      </c>
-      <c r="D1" s="69" t="s">
-        <v>277</v>
-      </c>
-      <c r="E1" s="69" t="s">
-        <v>278</v>
-      </c>
-      <c r="F1" s="69" t="s">
-        <v>279</v>
-      </c>
-      <c r="G1" s="69" t="s">
-        <v>280</v>
-      </c>
-      <c r="H1" s="69" t="s">
-        <v>281</v>
-      </c>
-      <c r="I1" s="69" t="s">
-        <v>282</v>
-      </c>
-      <c r="J1" s="69" t="s">
-        <v>283</v>
-      </c>
-      <c r="K1" s="69" t="s">
-        <v>284</v>
-      </c>
-      <c r="L1" s="69" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="68" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="42">
-        <v>0</v>
-      </c>
-      <c r="D2" s="42">
-        <v>0</v>
-      </c>
-      <c r="E2" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="F2" s="42">
-        <v>0</v>
-      </c>
-      <c r="G2" s="42">
-        <v>0</v>
-      </c>
-      <c r="H2" s="42">
-        <v>0</v>
-      </c>
-      <c r="I2" s="42">
-        <v>0</v>
-      </c>
-      <c r="J2" s="42">
-        <v>0</v>
-      </c>
-      <c r="K2" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="68" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="42">
-        <v>1</v>
-      </c>
-      <c r="D3" s="42">
-        <v>17.420000000000002</v>
-      </c>
-      <c r="E3" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="F3" s="42">
-        <v>0</v>
-      </c>
-      <c r="G3" s="42">
-        <v>0</v>
-      </c>
-      <c r="H3" s="42">
-        <v>0</v>
-      </c>
-      <c r="I3" s="42">
-        <v>0</v>
-      </c>
-      <c r="J3" s="42">
-        <v>17.420000000000002</v>
-      </c>
-      <c r="K3" s="42">
-        <v>5.23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="68" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="42">
-        <v>0</v>
-      </c>
-      <c r="D4" s="42">
-        <v>0</v>
-      </c>
-      <c r="E4" s="42">
-        <v>0.15</v>
-      </c>
-      <c r="F4" s="42">
-        <v>0</v>
-      </c>
-      <c r="G4" s="42">
-        <v>0</v>
-      </c>
-      <c r="H4" s="42">
-        <v>0</v>
-      </c>
-      <c r="I4" s="42">
-        <v>0</v>
-      </c>
-      <c r="J4" s="42">
-        <v>0</v>
-      </c>
-      <c r="K4" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="68" t="s">
-        <v>112</v>
-      </c>
-      <c r="B5" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="42">
-        <v>1</v>
-      </c>
-      <c r="D5" s="42">
-        <v>12.58</v>
-      </c>
-      <c r="E5" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="F5" s="42">
-        <v>0</v>
-      </c>
-      <c r="G5" s="42">
-        <v>0</v>
-      </c>
-      <c r="H5" s="42">
-        <v>1</v>
-      </c>
-      <c r="I5" s="42">
-        <v>2.09</v>
-      </c>
-      <c r="J5" s="42">
-        <v>12.58</v>
-      </c>
-      <c r="K5" s="42">
-        <v>5.87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="42">
-        <v>0</v>
-      </c>
-      <c r="D6" s="42">
-        <v>0</v>
-      </c>
-      <c r="E6" s="42">
-        <v>0.8</v>
-      </c>
-      <c r="F6" s="42">
-        <v>0</v>
-      </c>
-      <c r="G6" s="42">
-        <v>0</v>
-      </c>
-      <c r="H6" s="42">
-        <v>0</v>
-      </c>
-      <c r="I6" s="42">
-        <v>0</v>
-      </c>
-      <c r="J6" s="42">
-        <v>0</v>
-      </c>
-      <c r="K6" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="68" t="s">
-        <v>286</v>
-      </c>
-      <c r="B7" s="42" t="s">
-        <v>286</v>
-      </c>
-      <c r="C7" s="42">
-        <v>0</v>
-      </c>
-      <c r="E7" s="42">
-        <v>-1.2</v>
-      </c>
-      <c r="J7" s="42">
-        <v>0</v>
-      </c>
-      <c r="K7" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="68" t="s">
-        <v>162</v>
-      </c>
-      <c r="B8" s="42" t="s">
-        <v>162</v>
-      </c>
-      <c r="C8" s="42">
-        <v>1</v>
-      </c>
-      <c r="E8" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="J8" s="42">
-        <v>12.58</v>
-      </c>
-      <c r="K8" s="42">
-        <v>6.29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="42">
-        <v>1</v>
-      </c>
-      <c r="E9" s="42">
-        <v>0.15</v>
-      </c>
-      <c r="J9" s="42">
-        <v>17.420000000000002</v>
-      </c>
-      <c r="K9" s="42">
-        <v>2.61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="68" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="42">
-        <v>0</v>
-      </c>
-      <c r="E10" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="J10" s="42">
-        <v>0</v>
-      </c>
-      <c r="K10" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="68" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="42">
-        <v>0</v>
-      </c>
-      <c r="E11" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="J11" s="42">
-        <v>0</v>
-      </c>
-      <c r="K11" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="68" t="s">
-        <v>287</v>
-      </c>
-      <c r="K12" s="42">
-        <v>20</v>
-      </c>
-      <c r="L12" s="42">
-        <v>4567.28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:L12"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="15.85546875" style="42"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="69" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" s="69" t="s">
-        <v>276</v>
-      </c>
-      <c r="D1" s="69" t="s">
-        <v>277</v>
-      </c>
-      <c r="E1" s="69" t="s">
-        <v>278</v>
-      </c>
-      <c r="F1" s="69" t="s">
-        <v>279</v>
-      </c>
-      <c r="G1" s="69" t="s">
-        <v>280</v>
-      </c>
-      <c r="H1" s="69" t="s">
-        <v>281</v>
-      </c>
-      <c r="I1" s="69" t="s">
-        <v>282</v>
-      </c>
-      <c r="J1" s="69" t="s">
-        <v>283</v>
-      </c>
-      <c r="K1" s="69" t="s">
-        <v>284</v>
-      </c>
-      <c r="L1" s="69" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="68" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="42">
-        <v>0</v>
-      </c>
-      <c r="D2" s="42">
-        <v>0</v>
-      </c>
-      <c r="E2" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="F2" s="42">
-        <v>0</v>
-      </c>
-      <c r="G2" s="42">
-        <v>0</v>
-      </c>
-      <c r="H2" s="42">
-        <v>0</v>
-      </c>
-      <c r="I2" s="42">
-        <v>0</v>
-      </c>
-      <c r="J2" s="42">
-        <v>0</v>
-      </c>
-      <c r="K2" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="68" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="42">
-        <v>1</v>
-      </c>
-      <c r="D3" s="42">
-        <v>17.420000000000002</v>
-      </c>
-      <c r="E3" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="F3" s="42">
-        <v>0</v>
-      </c>
-      <c r="G3" s="42">
-        <v>0</v>
-      </c>
-      <c r="H3" s="42">
-        <v>0</v>
-      </c>
-      <c r="I3" s="42">
-        <v>0</v>
-      </c>
-      <c r="J3" s="42">
-        <v>17.420000000000002</v>
-      </c>
-      <c r="K3" s="42">
-        <v>5.23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="68" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="42">
-        <v>0</v>
-      </c>
-      <c r="D4" s="42">
-        <v>0</v>
-      </c>
-      <c r="E4" s="42">
-        <v>0.15</v>
-      </c>
-      <c r="F4" s="42">
-        <v>0</v>
-      </c>
-      <c r="G4" s="42">
-        <v>0</v>
-      </c>
-      <c r="H4" s="42">
-        <v>0</v>
-      </c>
-      <c r="I4" s="42">
-        <v>0</v>
-      </c>
-      <c r="J4" s="42">
-        <v>0</v>
-      </c>
-      <c r="K4" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="68" t="s">
-        <v>112</v>
-      </c>
-      <c r="B5" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="42">
-        <v>1</v>
-      </c>
-      <c r="D5" s="42">
-        <v>5.12</v>
-      </c>
-      <c r="E5" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="F5" s="42">
-        <v>1</v>
-      </c>
-      <c r="G5" s="42">
-        <v>3.04</v>
-      </c>
-      <c r="H5" s="42">
-        <v>1</v>
-      </c>
-      <c r="I5" s="42">
-        <v>2.09</v>
-      </c>
-      <c r="J5" s="42">
-        <v>4.33</v>
-      </c>
-      <c r="K5" s="42">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="42">
-        <v>1</v>
-      </c>
-      <c r="D6" s="42">
-        <v>17.45</v>
-      </c>
-      <c r="E6" s="42">
-        <v>0.8</v>
-      </c>
-      <c r="F6" s="42">
-        <v>1</v>
-      </c>
-      <c r="G6" s="42">
-        <v>17.45</v>
-      </c>
-      <c r="H6" s="42">
-        <v>0</v>
-      </c>
-      <c r="I6" s="42">
-        <v>0</v>
-      </c>
-      <c r="J6" s="42">
-        <v>12.91</v>
-      </c>
-      <c r="K6" s="42">
-        <v>1.1200000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="68" t="s">
-        <v>286</v>
-      </c>
-      <c r="B7" s="42" t="s">
-        <v>286</v>
-      </c>
-      <c r="C7" s="42">
-        <v>1</v>
-      </c>
-      <c r="E7" s="42">
-        <v>-1.2</v>
-      </c>
-      <c r="J7" s="42">
-        <v>5.33</v>
-      </c>
-      <c r="K7" s="42">
-        <v>-6.39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="68" t="s">
-        <v>162</v>
-      </c>
-      <c r="B8" s="42" t="s">
-        <v>162</v>
-      </c>
-      <c r="C8" s="42">
-        <v>1</v>
-      </c>
-      <c r="E8" s="42">
-        <v>0.45</v>
-      </c>
-      <c r="J8" s="42">
-        <v>22.58</v>
-      </c>
-      <c r="K8" s="42">
-        <v>10.16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="42">
-        <v>1</v>
-      </c>
-      <c r="E9" s="42">
-        <v>0.15</v>
-      </c>
-      <c r="J9" s="42">
-        <v>17.420000000000002</v>
-      </c>
-      <c r="K9" s="42">
-        <v>2.61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="68" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="42">
-        <v>0</v>
-      </c>
-      <c r="E10" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="J10" s="42">
-        <v>0</v>
-      </c>
-      <c r="K10" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="68" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="42">
-        <v>0</v>
-      </c>
-      <c r="E11" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="J11" s="42">
-        <v>0</v>
-      </c>
-      <c r="K11" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="68" t="s">
-        <v>287</v>
-      </c>
-      <c r="K12" s="42">
-        <v>13.47</v>
-      </c>
-      <c r="L12" s="42">
-        <v>3258.67</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
-  <dimension ref="A1:L12"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="15.5703125" style="42"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="69" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" s="69" t="s">
-        <v>276</v>
-      </c>
-      <c r="D1" s="69" t="s">
-        <v>277</v>
-      </c>
-      <c r="E1" s="69" t="s">
-        <v>278</v>
-      </c>
-      <c r="F1" s="69" t="s">
-        <v>279</v>
-      </c>
-      <c r="G1" s="69" t="s">
-        <v>280</v>
-      </c>
-      <c r="H1" s="69" t="s">
-        <v>281</v>
-      </c>
-      <c r="I1" s="69" t="s">
-        <v>282</v>
-      </c>
-      <c r="J1" s="69" t="s">
-        <v>283</v>
-      </c>
-      <c r="K1" s="69" t="s">
-        <v>284</v>
-      </c>
-      <c r="L1" s="69" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="68" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="42">
-        <v>0</v>
-      </c>
-      <c r="D2" s="42">
-        <v>0</v>
-      </c>
-      <c r="E2" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="F2" s="42">
-        <v>0</v>
-      </c>
-      <c r="G2" s="42">
-        <v>0</v>
-      </c>
-      <c r="H2" s="42">
-        <v>0</v>
-      </c>
-      <c r="I2" s="42">
-        <v>0</v>
-      </c>
-      <c r="J2" s="42">
-        <v>0</v>
-      </c>
-      <c r="K2" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="68" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="42">
-        <v>1</v>
-      </c>
-      <c r="D3" s="42">
-        <v>20.96</v>
-      </c>
-      <c r="E3" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="F3" s="42">
-        <v>0</v>
-      </c>
-      <c r="G3" s="42">
-        <v>0</v>
-      </c>
-      <c r="H3" s="42">
-        <v>0</v>
-      </c>
-      <c r="I3" s="42">
-        <v>0</v>
-      </c>
-      <c r="J3" s="42">
-        <v>20.96</v>
-      </c>
-      <c r="K3" s="42">
-        <v>6.29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="68" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="42">
-        <v>0</v>
-      </c>
-      <c r="D4" s="42">
-        <v>0</v>
-      </c>
-      <c r="E4" s="42">
-        <v>0.15</v>
-      </c>
-      <c r="F4" s="42">
-        <v>0</v>
-      </c>
-      <c r="G4" s="42">
-        <v>0</v>
-      </c>
-      <c r="H4" s="42">
-        <v>0</v>
-      </c>
-      <c r="I4" s="42">
-        <v>0</v>
-      </c>
-      <c r="J4" s="42">
-        <v>0</v>
-      </c>
-      <c r="K4" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="68" t="s">
-        <v>112</v>
-      </c>
-      <c r="B5" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="42">
-        <v>1</v>
-      </c>
-      <c r="D5" s="42">
-        <v>10.84</v>
-      </c>
-      <c r="E5" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="F5" s="42">
-        <v>1</v>
-      </c>
-      <c r="G5" s="42">
-        <v>8.75</v>
-      </c>
-      <c r="H5" s="42">
-        <v>1</v>
-      </c>
-      <c r="I5" s="42">
-        <v>2.09</v>
-      </c>
-      <c r="J5" s="42">
-        <v>8.56</v>
-      </c>
-      <c r="K5" s="42">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="42">
-        <v>1</v>
-      </c>
-      <c r="D6" s="42">
-        <v>18.2</v>
-      </c>
-      <c r="E6" s="42">
-        <v>0.8</v>
-      </c>
-      <c r="F6" s="42">
-        <v>1</v>
-      </c>
-      <c r="G6" s="42">
-        <v>18.2</v>
-      </c>
-      <c r="H6" s="42">
-        <v>0</v>
-      </c>
-      <c r="I6" s="42">
-        <v>0</v>
-      </c>
-      <c r="J6" s="42">
-        <v>13.47</v>
-      </c>
-      <c r="K6" s="42">
-        <v>1.1599999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="68" t="s">
-        <v>286</v>
-      </c>
-      <c r="B7" s="42" t="s">
-        <v>286</v>
-      </c>
-      <c r="C7" s="42">
-        <v>1</v>
-      </c>
-      <c r="E7" s="42">
-        <v>-1.2</v>
-      </c>
-      <c r="J7" s="42">
-        <v>10.55</v>
-      </c>
-      <c r="K7" s="42">
-        <v>-12.66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="68" t="s">
-        <v>162</v>
-      </c>
-      <c r="B8" s="42" t="s">
-        <v>162</v>
-      </c>
-      <c r="C8" s="42">
-        <v>1</v>
-      </c>
-      <c r="E8" s="42">
-        <v>0.4</v>
-      </c>
-      <c r="J8" s="42">
-        <v>29.04</v>
-      </c>
-      <c r="K8" s="42">
-        <v>11.61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="42">
-        <v>1</v>
-      </c>
-      <c r="E9" s="42">
-        <v>0.15</v>
-      </c>
-      <c r="J9" s="42">
-        <v>17.420000000000002</v>
-      </c>
-      <c r="K9" s="42">
-        <v>2.61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="68" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="42">
-        <v>0</v>
-      </c>
-      <c r="E10" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="J10" s="42">
-        <v>0</v>
-      </c>
-      <c r="K10" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="68" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="42">
-        <v>0</v>
-      </c>
-      <c r="E11" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="J11" s="42">
-        <v>0</v>
-      </c>
-      <c r="K11" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="68" t="s">
-        <v>287</v>
-      </c>
-      <c r="K12" s="42">
-        <v>10</v>
-      </c>
-      <c r="L12" s="42">
-        <v>3907.62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
-  <dimension ref="A1:L12"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="15.7109375" style="42"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="69" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" s="69" t="s">
-        <v>276</v>
-      </c>
-      <c r="D1" s="69" t="s">
-        <v>277</v>
-      </c>
-      <c r="E1" s="69" t="s">
-        <v>278</v>
-      </c>
-      <c r="F1" s="69" t="s">
-        <v>279</v>
-      </c>
-      <c r="G1" s="69" t="s">
-        <v>280</v>
-      </c>
-      <c r="H1" s="69" t="s">
-        <v>281</v>
-      </c>
-      <c r="I1" s="69" t="s">
-        <v>282</v>
-      </c>
-      <c r="J1" s="69" t="s">
-        <v>283</v>
-      </c>
-      <c r="K1" s="69" t="s">
-        <v>284</v>
-      </c>
-      <c r="L1" s="69" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="68" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="42">
-        <v>0</v>
-      </c>
-      <c r="D2" s="42">
-        <v>0</v>
-      </c>
-      <c r="E2" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="F2" s="42">
-        <v>0</v>
-      </c>
-      <c r="G2" s="42">
-        <v>0</v>
-      </c>
-      <c r="H2" s="42">
-        <v>0</v>
-      </c>
-      <c r="I2" s="42">
-        <v>0</v>
-      </c>
-      <c r="J2" s="42">
-        <v>0</v>
-      </c>
-      <c r="K2" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="68" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="42">
-        <v>1</v>
-      </c>
-      <c r="D3" s="42">
-        <v>21.3</v>
-      </c>
-      <c r="E3" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="F3" s="42">
-        <v>0</v>
-      </c>
-      <c r="G3" s="42">
-        <v>0</v>
-      </c>
-      <c r="H3" s="42">
-        <v>0</v>
-      </c>
-      <c r="I3" s="42">
-        <v>0</v>
-      </c>
-      <c r="J3" s="42">
-        <v>21.3</v>
-      </c>
-      <c r="K3" s="42">
-        <v>6.39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="68" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="42">
-        <v>1</v>
-      </c>
-      <c r="D4" s="42">
-        <v>20</v>
-      </c>
-      <c r="E4" s="42">
-        <v>0.15</v>
-      </c>
-      <c r="F4" s="42">
-        <v>0</v>
-      </c>
-      <c r="G4" s="42">
-        <v>0</v>
-      </c>
-      <c r="H4" s="42">
-        <v>0</v>
-      </c>
-      <c r="I4" s="42">
-        <v>0</v>
-      </c>
-      <c r="J4" s="42">
-        <v>20</v>
-      </c>
-      <c r="K4" s="42">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="68" t="s">
-        <v>112</v>
-      </c>
-      <c r="B5" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="42">
-        <v>1</v>
-      </c>
-      <c r="D5" s="42">
-        <v>20.5</v>
-      </c>
-      <c r="E5" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="F5" s="42">
-        <v>1</v>
-      </c>
-      <c r="G5" s="42">
-        <v>18.41</v>
-      </c>
-      <c r="H5" s="42">
-        <v>1</v>
-      </c>
-      <c r="I5" s="42">
-        <v>2.09</v>
-      </c>
-      <c r="J5" s="42">
-        <v>15.71</v>
-      </c>
-      <c r="K5" s="42">
-        <v>1.36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="42">
-        <v>1</v>
-      </c>
-      <c r="D6" s="42">
-        <v>18.2</v>
-      </c>
-      <c r="E6" s="42">
-        <v>0.8</v>
-      </c>
-      <c r="F6" s="42">
-        <v>1</v>
-      </c>
-      <c r="G6" s="42">
-        <v>18.2</v>
-      </c>
-      <c r="H6" s="42">
-        <v>0</v>
-      </c>
-      <c r="I6" s="42">
-        <v>0</v>
-      </c>
-      <c r="J6" s="42">
-        <v>13.47</v>
-      </c>
-      <c r="K6" s="42">
-        <v>1.1599999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="68" t="s">
-        <v>286</v>
-      </c>
-      <c r="B7" s="42" t="s">
-        <v>286</v>
-      </c>
-      <c r="C7" s="42">
-        <v>1</v>
-      </c>
-      <c r="E7" s="42">
-        <v>-1.2</v>
-      </c>
-      <c r="J7" s="42">
-        <v>13.4</v>
-      </c>
-      <c r="K7" s="42">
-        <v>-16.079999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="68" t="s">
-        <v>162</v>
-      </c>
-      <c r="B8" s="42" t="s">
-        <v>162</v>
-      </c>
-      <c r="C8" s="42">
-        <v>1</v>
-      </c>
-      <c r="E8" s="42">
-        <v>0.35</v>
-      </c>
-      <c r="J8" s="42">
-        <v>18.7</v>
-      </c>
-      <c r="K8" s="42">
-        <v>6.54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="42">
-        <v>1</v>
-      </c>
-      <c r="E9" s="42">
-        <v>0.15</v>
-      </c>
-      <c r="J9" s="42">
-        <v>17.420000000000002</v>
-      </c>
-      <c r="K9" s="42">
-        <v>2.61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="68" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="42">
-        <v>0</v>
-      </c>
-      <c r="E10" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="J10" s="42">
-        <v>0</v>
-      </c>
-      <c r="K10" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="68" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="42">
-        <v>0</v>
-      </c>
-      <c r="E11" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="J11" s="42">
-        <v>0</v>
-      </c>
-      <c r="K11" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="68" t="s">
-        <v>287</v>
-      </c>
-      <c r="K12" s="42">
-        <v>5</v>
-      </c>
-      <c r="L12" s="42">
-        <v>5003.3100000000004</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -9067,6 +6961,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="H2:I2"/>
@@ -9075,11 +6974,6 @@
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="A12:I12"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -10301,17 +8195,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="A20:O20"/>
@@ -10320,6 +8203,17 @@
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="H4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -10946,17 +8840,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="A20:O20"/>
@@ -10965,6 +8848,17 @@
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="H4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>